<commit_message>
GIZ-00: update test excels
</commit_message>
<xml_diff>
--- a/test/import-excels/giz-calc-1w-100perc-20gap.xlsx
+++ b/test/import-excels/giz-calc-1w-100perc-20gap.xlsx
@@ -24,7 +24,7 @@
     <t>Facility name</t>
   </si>
   <si>
-    <t>Calculation test round numbers single worker</t>
+    <t>Calc Test - 1w 100perc 20gap</t>
   </si>
   <si>
     <t>Facility id</t>
@@ -36,7 +36,7 @@
     <t>Salary matrix manager</t>
   </si>
   <si>
-    <t>Juan  Stelling</t>
+    <t>anonymous</t>
   </si>
   <si>
     <t>Phone number</t>
@@ -45,7 +45,15 @@
     <t>Email</t>
   </si>
   <si>
-    <t>juan.stelling@usmedia.nl</t>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>anonymous@sample.com</t>
+    </r>
   </si>
   <si>
     <t>Facility country</t>
@@ -63,9 +71,6 @@
     <t>Facility location</t>
   </si>
   <si>
-    <t>10.083619,	-83.330709</t>
-  </si>
-  <si>
     <t>Total Facility Living Wage Gap</t>
   </si>
   <si>
@@ -120,202 +125,205 @@
     <t>Benchmark</t>
   </si>
   <si>
+    <t>2022 - anker - Rural, Benchmark Test 4</t>
+  </si>
+  <si>
+    <t>Finalized date</t>
+  </si>
+  <si>
+    <t>Version</t>
+  </si>
+  <si>
+    <t>2.2.0</t>
+  </si>
+  <si>
+    <t>Number of registered trade unions active</t>
+  </si>
+  <si>
+    <t>Are workers presented by another type of worker organisation (Yes, No)</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Number of hours of unpaid mandatory leave</t>
+  </si>
+  <si>
+    <t>0.0000</t>
+  </si>
+  <si>
+    <t>Number of hours of paid annual leave</t>
+  </si>
+  <si>
+    <t>Number of workers employed via 3rd party</t>
+  </si>
+  <si>
+    <t>Is there any work performed by subcontractors (Yes, No)</t>
+  </si>
+  <si>
+    <t>Number of workers paid, partially or totally, by piece-rate</t>
+  </si>
+  <si>
+    <t>note</t>
+  </si>
+  <si>
+    <t>Not all values could be filled because this matrix is not submitted yet.</t>
+  </si>
+  <si>
+    <t>Workers</t>
+  </si>
+  <si>
+    <t>Work type/duration</t>
+  </si>
+  <si>
+    <t>Work Area</t>
+  </si>
+  <si>
+    <t>Job Category</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>Employees</t>
+  </si>
+  <si>
+    <t>Bonus 13th 14th month</t>
+  </si>
+  <si>
+    <t>Other bonus 1</t>
+  </si>
+  <si>
+    <t>Other bonus 2</t>
+  </si>
+  <si>
+    <t>Other bonus 3</t>
+  </si>
+  <si>
+    <t>Bonus total monthly</t>
+  </si>
+  <si>
+    <t>S1 hours worked</t>
+  </si>
+  <si>
+    <t>S1 wage earned</t>
+  </si>
+  <si>
+    <t>S1 hours worked in overtime</t>
+  </si>
+  <si>
+    <t>S1 wage earned in overtime</t>
+  </si>
+  <si>
+    <t>S2 hours worked</t>
+  </si>
+  <si>
+    <t>S2 wage earned</t>
+  </si>
+  <si>
+    <t>S2 hours worked in overtime</t>
+  </si>
+  <si>
+    <t>S2 wage earned in overtime</t>
+  </si>
+  <si>
+    <t>S3 hours worked</t>
+  </si>
+  <si>
+    <t>S3 wage earned</t>
+  </si>
+  <si>
+    <t>S3 hours worked in overtime</t>
+  </si>
+  <si>
+    <t>S3 wage earned in overtime</t>
+  </si>
+  <si>
+    <t>In Kind Benefits Food</t>
+  </si>
+  <si>
+    <t>In Kind Benefits Transportation</t>
+  </si>
+  <si>
+    <t>In Kind Benefits Housing</t>
+  </si>
+  <si>
+    <t>In Kind Benefits Healthcare</t>
+  </si>
+  <si>
+    <t>In Kind Benefits Child education</t>
+  </si>
+  <si>
+    <t>In Kind Benefits Child Care</t>
+  </si>
+  <si>
+    <t>Monthly In Kind Benefits</t>
+  </si>
+  <si>
+    <t>Monthly In Kind Benefits capped</t>
+  </si>
+  <si>
+    <t>Average wage per month adjusted for average working week</t>
+  </si>
+  <si>
+    <t>Total value of bonus monthly</t>
+  </si>
+  <si>
+    <t>Total monthly remuneration</t>
+  </si>
+  <si>
+    <t>Percentage of year worked</t>
+  </si>
+  <si>
+    <t>Applicable benchmark name</t>
+  </si>
+  <si>
+    <t>Benchmark value</t>
+  </si>
+  <si>
+    <t>Living wage gap</t>
+  </si>
+  <si>
+    <t>Living wage gap as percentage</t>
+  </si>
+  <si>
+    <t>Lowest payed job category / worker</t>
+  </si>
+  <si>
+    <t>Lowest payed worker total remuneration</t>
+  </si>
+  <si>
+    <t>Years of tenure</t>
+  </si>
+  <si>
+    <t>A portion of the year - Full-time</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>00021CAL</t>
+  </si>
+  <si>
+    <t>Men</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>0.00</t>
+  </si>
+  <si>
+    <t>5000.00</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>100.00%</t>
+  </si>
+  <si>
     <t>2022 - anker - Rural, Limon and Heredia Provinces</t>
-  </si>
-  <si>
-    <t>Finalized date</t>
-  </si>
-  <si>
-    <t>Version</t>
-  </si>
-  <si>
-    <t>2.2.0</t>
-  </si>
-  <si>
-    <t>Number of registered trade unions active</t>
-  </si>
-  <si>
-    <t>Are workers presented by another type of worker organisation (Yes, No)</t>
-  </si>
-  <si>
-    <t>Yes</t>
-  </si>
-  <si>
-    <t>Number of hours of unpaid mandatory leave</t>
-  </si>
-  <si>
-    <t>0.0000</t>
-  </si>
-  <si>
-    <t>Number of hours of paid annual leave</t>
-  </si>
-  <si>
-    <t>Number of workers employed via 3rd party</t>
-  </si>
-  <si>
-    <t>Is there any work performed by subcontractors (Yes, No)</t>
-  </si>
-  <si>
-    <t>Number of workers paid, partially or totally, by piece-rate</t>
-  </si>
-  <si>
-    <t>note</t>
-  </si>
-  <si>
-    <t>Not all values could be filled because this matrix is not submitted yet.</t>
-  </si>
-  <si>
-    <t>Workers</t>
-  </si>
-  <si>
-    <t>Work type/duration</t>
-  </si>
-  <si>
-    <t>Work Area</t>
-  </si>
-  <si>
-    <t>Job Category</t>
-  </si>
-  <si>
-    <t>Gender</t>
-  </si>
-  <si>
-    <t>Employees</t>
-  </si>
-  <si>
-    <t>Bonus 13th 14th month</t>
-  </si>
-  <si>
-    <t>Other bonus 1</t>
-  </si>
-  <si>
-    <t>Other bonus 2</t>
-  </si>
-  <si>
-    <t>Other bonus 3</t>
-  </si>
-  <si>
-    <t>Bonus total monthly</t>
-  </si>
-  <si>
-    <t>S1 hours worked</t>
-  </si>
-  <si>
-    <t>S1 wage earned</t>
-  </si>
-  <si>
-    <t>S1 hours worked in overtime</t>
-  </si>
-  <si>
-    <t>S1 wage earned in overtime</t>
-  </si>
-  <si>
-    <t>S2 hours worked</t>
-  </si>
-  <si>
-    <t>S2 wage earned</t>
-  </si>
-  <si>
-    <t>S2 hours worked in overtime</t>
-  </si>
-  <si>
-    <t>S2 wage earned in overtime</t>
-  </si>
-  <si>
-    <t>S3 hours worked</t>
-  </si>
-  <si>
-    <t>S3 wage earned</t>
-  </si>
-  <si>
-    <t>S3 hours worked in overtime</t>
-  </si>
-  <si>
-    <t>S3 wage earned in overtime</t>
-  </si>
-  <si>
-    <t>In Kind Benefits Food</t>
-  </si>
-  <si>
-    <t>In Kind Benefits Transportation</t>
-  </si>
-  <si>
-    <t>In Kind Benefits Housing</t>
-  </si>
-  <si>
-    <t>In Kind Benefits Healthcare</t>
-  </si>
-  <si>
-    <t>In Kind Benefits Child education</t>
-  </si>
-  <si>
-    <t>In Kind Benefits Child Care</t>
-  </si>
-  <si>
-    <t>Monthly In Kind Benefits</t>
-  </si>
-  <si>
-    <t>Monthly In Kind Benefits capped</t>
-  </si>
-  <si>
-    <t>Average wage per month adjusted for average working week</t>
-  </si>
-  <si>
-    <t>Total value of bonus monthly</t>
-  </si>
-  <si>
-    <t>Total monthly remuneration</t>
-  </si>
-  <si>
-    <t>Percentage of year worked</t>
-  </si>
-  <si>
-    <t>Applicable benchmark name</t>
-  </si>
-  <si>
-    <t>Benchmark value</t>
-  </si>
-  <si>
-    <t>Living wage gap</t>
-  </si>
-  <si>
-    <t>Living wage gap as percentage</t>
-  </si>
-  <si>
-    <t>Lowest payed job category / worker</t>
-  </si>
-  <si>
-    <t>Lowest payed worker total remuneration</t>
-  </si>
-  <si>
-    <t>Years of tenure</t>
-  </si>
-  <si>
-    <t>A portion of the year - Full-time</t>
-  </si>
-  <si>
-    <t>Other</t>
-  </si>
-  <si>
-    <t>00021CAL</t>
-  </si>
-  <si>
-    <t>Men</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>0.00</t>
-  </si>
-  <si>
-    <t>5000.00</t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t>100.00%</t>
   </si>
   <si>
     <t>6000.00</t>
@@ -349,7 +357,7 @@
   <numFmts count="1">
     <numFmt numFmtId="0" formatCode="General"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -363,6 +371,12 @@
     <font>
       <sz val="15"/>
       <color indexed="8"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <u val="single"/>
+      <sz val="11"/>
+      <color indexed="11"/>
       <name val="Calibri"/>
     </font>
   </fonts>
@@ -380,7 +394,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -501,7 +515,7 @@
         <color indexed="10"/>
       </top>
       <bottom style="medium">
-        <color indexed="11"/>
+        <color indexed="12"/>
       </bottom>
       <diagonal/>
     </border>
@@ -509,8 +523,39 @@
       <left style="thin">
         <color indexed="10"/>
       </left>
+      <right/>
+      <top style="medium">
+        <color indexed="12"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="12"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="medium">
+        <color indexed="12"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
       <right style="medium">
-        <color indexed="11"/>
+        <color indexed="12"/>
       </right>
       <top style="thin">
         <color indexed="10"/>
@@ -522,10 +567,10 @@
     </border>
     <border>
       <left style="medium">
-        <color indexed="11"/>
+        <color indexed="12"/>
       </left>
       <right style="medium">
-        <color indexed="11"/>
+        <color indexed="12"/>
       </right>
       <top style="thin">
         <color indexed="10"/>
@@ -540,13 +585,13 @@
         <color indexed="10"/>
       </left>
       <right style="medium">
-        <color indexed="11"/>
+        <color indexed="12"/>
       </right>
       <top style="thin">
         <color indexed="10"/>
       </top>
       <bottom style="medium">
-        <color indexed="11"/>
+        <color indexed="12"/>
       </bottom>
       <diagonal/>
     </border>
@@ -558,7 +603,7 @@
         <color indexed="10"/>
       </right>
       <top style="medium">
-        <color indexed="11"/>
+        <color indexed="12"/>
       </top>
       <bottom style="thin">
         <color indexed="10"/>
@@ -570,10 +615,10 @@
         <color indexed="10"/>
       </left>
       <right style="medium">
-        <color indexed="11"/>
+        <color indexed="12"/>
       </right>
       <top style="medium">
-        <color indexed="11"/>
+        <color indexed="12"/>
       </top>
       <bottom style="thin">
         <color indexed="10"/>
@@ -586,7 +631,7 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -653,31 +698,46 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="15" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -699,6 +759,7 @@
       <rgbColor rgb="ff000000"/>
       <rgbColor rgb="ffffffff"/>
       <rgbColor rgb="ffaaaaaa"/>
+      <rgbColor rgb="ff0000ff"/>
       <rgbColor rgb="ffb2b2b2"/>
     </indexedColors>
   </colors>
@@ -1862,19 +1923,17 @@
       <c r="A9" t="s" s="6">
         <v>15</v>
       </c>
-      <c r="B9" t="s" s="7">
-        <v>16</v>
-      </c>
+      <c r="B9" s="7"/>
       <c r="C9" s="8"/>
       <c r="D9" s="8"/>
       <c r="E9" s="9"/>
     </row>
     <row r="10" ht="13.55" customHeight="1">
       <c r="A10" t="s" s="6">
+        <v>16</v>
+      </c>
+      <c r="B10" t="s" s="7">
         <v>17</v>
-      </c>
-      <c r="B10" t="s" s="7">
-        <v>18</v>
       </c>
       <c r="C10" s="8"/>
       <c r="D10" s="8"/>
@@ -1882,10 +1941,10 @@
     </row>
     <row r="11" ht="13.55" customHeight="1">
       <c r="A11" t="s" s="6">
+        <v>18</v>
+      </c>
+      <c r="B11" t="s" s="7">
         <v>19</v>
-      </c>
-      <c r="B11" t="s" s="7">
-        <v>20</v>
       </c>
       <c r="C11" s="8"/>
       <c r="D11" s="8"/>
@@ -1893,7 +1952,7 @@
     </row>
     <row r="12" ht="13.55" customHeight="1">
       <c r="A12" t="s" s="6">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B12" s="8"/>
       <c r="C12" s="8"/>
@@ -1902,10 +1961,10 @@
     </row>
     <row r="13" ht="13.55" customHeight="1">
       <c r="A13" t="s" s="6">
+        <v>21</v>
+      </c>
+      <c r="B13" t="s" s="7">
         <v>22</v>
-      </c>
-      <c r="B13" t="s" s="7">
-        <v>23</v>
       </c>
       <c r="C13" s="8"/>
       <c r="D13" s="8"/>
@@ -1913,10 +1972,10 @@
     </row>
     <row r="14" ht="13.55" customHeight="1">
       <c r="A14" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="B14" t="s" s="7">
         <v>24</v>
-      </c>
-      <c r="B14" t="s" s="7">
-        <v>25</v>
       </c>
       <c r="C14" s="8"/>
       <c r="D14" s="8"/>
@@ -1924,7 +1983,7 @@
     </row>
     <row r="15" ht="13.55" customHeight="1">
       <c r="A15" t="s" s="6">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B15" s="8"/>
       <c r="C15" s="8"/>
@@ -1933,10 +1992,10 @@
     </row>
     <row r="16" ht="13.55" customHeight="1">
       <c r="A16" t="s" s="6">
+        <v>26</v>
+      </c>
+      <c r="B16" t="s" s="7">
         <v>27</v>
-      </c>
-      <c r="B16" t="s" s="7">
-        <v>28</v>
       </c>
       <c r="C16" s="8"/>
       <c r="D16" s="8"/>
@@ -1944,10 +2003,10 @@
     </row>
     <row r="17" ht="13.55" customHeight="1">
       <c r="A17" t="s" s="6">
+        <v>28</v>
+      </c>
+      <c r="B17" t="s" s="7">
         <v>29</v>
-      </c>
-      <c r="B17" t="s" s="7">
-        <v>30</v>
       </c>
       <c r="C17" s="8"/>
       <c r="D17" s="8"/>
@@ -1955,7 +2014,7 @@
     </row>
     <row r="18" ht="13.55" customHeight="1">
       <c r="A18" t="s" s="6">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B18" s="10">
         <v>2022</v>
@@ -1966,10 +2025,10 @@
     </row>
     <row r="19" ht="13.55" customHeight="1">
       <c r="A19" t="s" s="6">
+        <v>31</v>
+      </c>
+      <c r="B19" t="s" s="7">
         <v>32</v>
-      </c>
-      <c r="B19" t="s" s="7">
-        <v>33</v>
       </c>
       <c r="C19" s="8"/>
       <c r="D19" s="8"/>
@@ -1977,10 +2036,10 @@
     </row>
     <row r="20" ht="13.55" customHeight="1">
       <c r="A20" t="s" s="6">
+        <v>33</v>
+      </c>
+      <c r="B20" t="s" s="7">
         <v>34</v>
-      </c>
-      <c r="B20" t="s" s="7">
-        <v>35</v>
       </c>
       <c r="C20" s="8"/>
       <c r="D20" s="8"/>
@@ -1988,7 +2047,7 @@
     </row>
     <row r="21" ht="13.55" customHeight="1">
       <c r="A21" t="s" s="6">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B21" s="8"/>
       <c r="C21" s="8"/>
@@ -1997,10 +2056,10 @@
     </row>
     <row r="22" ht="13.55" customHeight="1">
       <c r="A22" t="s" s="6">
+        <v>36</v>
+      </c>
+      <c r="B22" t="s" s="7">
         <v>37</v>
-      </c>
-      <c r="B22" t="s" s="7">
-        <v>38</v>
       </c>
       <c r="C22" s="8"/>
       <c r="D22" s="8"/>
@@ -2008,7 +2067,7 @@
     </row>
     <row r="23" ht="13.55" customHeight="1">
       <c r="A23" t="s" s="6">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B23" s="10">
         <v>3</v>
@@ -2019,10 +2078,10 @@
     </row>
     <row r="24" ht="13.55" customHeight="1">
       <c r="A24" t="s" s="6">
+        <v>39</v>
+      </c>
+      <c r="B24" t="s" s="7">
         <v>40</v>
-      </c>
-      <c r="B24" t="s" s="7">
-        <v>41</v>
       </c>
       <c r="C24" s="8"/>
       <c r="D24" s="8"/>
@@ -2030,10 +2089,10 @@
     </row>
     <row r="25" ht="13.55" customHeight="1">
       <c r="A25" t="s" s="6">
+        <v>41</v>
+      </c>
+      <c r="B25" t="s" s="7">
         <v>42</v>
-      </c>
-      <c r="B25" t="s" s="7">
-        <v>43</v>
       </c>
       <c r="C25" s="8"/>
       <c r="D25" s="8"/>
@@ -2041,10 +2100,10 @@
     </row>
     <row r="26" ht="13.55" customHeight="1">
       <c r="A26" t="s" s="6">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B26" t="s" s="7">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C26" s="8"/>
       <c r="D26" s="8"/>
@@ -2052,7 +2111,7 @@
     </row>
     <row r="27" ht="13.55" customHeight="1">
       <c r="A27" t="s" s="6">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B27" s="10">
         <v>0</v>
@@ -2063,10 +2122,10 @@
     </row>
     <row r="28" ht="13.55" customHeight="1">
       <c r="A28" t="s" s="6">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B28" t="s" s="7">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C28" s="8"/>
       <c r="D28" s="8"/>
@@ -2074,7 +2133,7 @@
     </row>
     <row r="29" ht="13.55" customHeight="1">
       <c r="A29" t="s" s="6">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B29" s="10">
         <v>346</v>
@@ -2085,16 +2144,19 @@
     </row>
     <row r="30" ht="13.55" customHeight="1">
       <c r="A30" t="s" s="11">
+        <v>47</v>
+      </c>
+      <c r="B30" t="s" s="12">
         <v>48</v>
-      </c>
-      <c r="B30" t="s" s="12">
-        <v>49</v>
       </c>
       <c r="C30" s="13"/>
       <c r="D30" s="13"/>
       <c r="E30" s="14"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B6" r:id="rId1" location="" tooltip="" display="anonymous@sample.com"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
   <headerFooter>
@@ -2105,7 +2167,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:BD4"/>
+  <dimension ref="A1:BD10"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -2152,7 +2214,7 @@
   <sheetData>
     <row r="1" ht="20" customHeight="1">
       <c r="A1" t="s" s="16">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B1" s="17"/>
       <c r="C1" s="17"/>
@@ -2212,142 +2274,142 @@
     </row>
     <row r="2" ht="13.55" customHeight="1">
       <c r="A2" t="s" s="19">
+        <v>50</v>
+      </c>
+      <c r="B2" t="s" s="19">
         <v>51</v>
       </c>
-      <c r="B2" t="s" s="19">
+      <c r="C2" t="s" s="19">
         <v>52</v>
       </c>
-      <c r="C2" t="s" s="19">
+      <c r="D2" t="s" s="19">
         <v>53</v>
       </c>
-      <c r="D2" t="s" s="19">
+      <c r="E2" t="s" s="19">
         <v>54</v>
-      </c>
-      <c r="E2" t="s" s="19">
-        <v>55</v>
       </c>
       <c r="F2" s="18"/>
       <c r="G2" t="s" s="19">
+        <v>55</v>
+      </c>
+      <c r="H2" t="s" s="19">
         <v>56</v>
       </c>
-      <c r="H2" t="s" s="19">
+      <c r="I2" t="s" s="19">
         <v>57</v>
       </c>
-      <c r="I2" t="s" s="19">
+      <c r="J2" t="s" s="19">
         <v>58</v>
       </c>
-      <c r="J2" t="s" s="19">
+      <c r="K2" t="s" s="19">
         <v>59</v>
-      </c>
-      <c r="K2" t="s" s="19">
-        <v>60</v>
       </c>
       <c r="L2" s="18"/>
       <c r="M2" t="s" s="19">
+        <v>60</v>
+      </c>
+      <c r="N2" t="s" s="19">
         <v>61</v>
       </c>
-      <c r="N2" t="s" s="19">
+      <c r="O2" t="s" s="19">
         <v>62</v>
       </c>
-      <c r="O2" t="s" s="19">
+      <c r="P2" t="s" s="19">
         <v>63</v>
-      </c>
-      <c r="P2" t="s" s="19">
-        <v>64</v>
       </c>
       <c r="Q2" s="18"/>
       <c r="R2" t="s" s="19">
+        <v>64</v>
+      </c>
+      <c r="S2" t="s" s="19">
         <v>65</v>
       </c>
-      <c r="S2" t="s" s="19">
+      <c r="T2" t="s" s="19">
         <v>66</v>
       </c>
-      <c r="T2" t="s" s="19">
+      <c r="U2" t="s" s="19">
         <v>67</v>
-      </c>
-      <c r="U2" t="s" s="19">
-        <v>68</v>
       </c>
       <c r="V2" s="18"/>
       <c r="W2" t="s" s="19">
+        <v>68</v>
+      </c>
+      <c r="X2" t="s" s="19">
         <v>69</v>
       </c>
-      <c r="X2" t="s" s="19">
+      <c r="Y2" t="s" s="19">
         <v>70</v>
       </c>
-      <c r="Y2" t="s" s="19">
+      <c r="Z2" t="s" s="19">
         <v>71</v>
-      </c>
-      <c r="Z2" t="s" s="19">
-        <v>72</v>
       </c>
       <c r="AA2" s="18"/>
       <c r="AB2" t="s" s="19">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="AC2" s="18"/>
       <c r="AD2" t="s" s="19">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="AE2" s="18"/>
       <c r="AF2" t="s" s="19">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="AG2" s="18"/>
       <c r="AH2" t="s" s="19">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="AI2" s="18"/>
       <c r="AJ2" t="s" s="19">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AK2" s="18"/>
       <c r="AL2" t="s" s="19">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AM2" s="18"/>
       <c r="AN2" t="s" s="19">
+        <v>78</v>
+      </c>
+      <c r="AO2" t="s" s="19">
         <v>79</v>
-      </c>
-      <c r="AO2" t="s" s="19">
-        <v>80</v>
       </c>
       <c r="AP2" s="18"/>
       <c r="AQ2" t="s" s="19">
+        <v>80</v>
+      </c>
+      <c r="AR2" t="s" s="19">
         <v>81</v>
       </c>
-      <c r="AR2" t="s" s="19">
+      <c r="AS2" t="s" s="19">
         <v>82</v>
       </c>
-      <c r="AS2" t="s" s="19">
+      <c r="AT2" t="s" s="19">
         <v>83</v>
-      </c>
-      <c r="AT2" t="s" s="19">
-        <v>84</v>
       </c>
       <c r="AU2" s="18"/>
       <c r="AV2" t="s" s="19">
+        <v>84</v>
+      </c>
+      <c r="AW2" t="s" s="19">
         <v>85</v>
       </c>
-      <c r="AW2" t="s" s="19">
+      <c r="AX2" t="s" s="19">
         <v>86</v>
       </c>
-      <c r="AX2" t="s" s="19">
+      <c r="AY2" t="s" s="19">
         <v>87</v>
-      </c>
-      <c r="AY2" t="s" s="19">
-        <v>88</v>
       </c>
       <c r="AZ2" s="18"/>
       <c r="BA2" t="s" s="19">
+        <v>88</v>
+      </c>
+      <c r="BB2" t="s" s="19">
         <v>89</v>
-      </c>
-      <c r="BB2" t="s" s="19">
-        <v>90</v>
       </c>
       <c r="BC2" s="18"/>
       <c r="BD2" t="s" s="19">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="3" ht="10" customHeight="1">
@@ -2410,48 +2472,48 @@
     </row>
     <row r="4" ht="20" customHeight="1">
       <c r="A4" t="s" s="20">
+        <v>91</v>
+      </c>
+      <c r="B4" t="s" s="20">
         <v>92</v>
       </c>
-      <c r="B4" t="s" s="20">
+      <c r="C4" t="s" s="20">
         <v>93</v>
       </c>
-      <c r="C4" t="s" s="20">
+      <c r="D4" t="s" s="20">
         <v>94</v>
       </c>
-      <c r="D4" t="s" s="20">
+      <c r="E4" t="s" s="20">
         <v>95</v>
-      </c>
-      <c r="E4" t="s" s="20">
-        <v>96</v>
       </c>
       <c r="F4" s="18"/>
       <c r="G4" t="s" s="20">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H4" t="s" s="20">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I4" t="s" s="20">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="J4" t="s" s="20">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="K4" t="s" s="20">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="L4" s="18"/>
       <c r="M4" t="s" s="20">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="N4" t="s" s="20">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="O4" t="s" s="20">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="P4" t="s" s="20">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="Q4" s="18"/>
       <c r="R4" s="18"/>
@@ -2465,72 +2527,420 @@
       <c r="Z4" s="18"/>
       <c r="AA4" s="18"/>
       <c r="AB4" t="s" s="20">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="AC4" s="18"/>
       <c r="AD4" t="s" s="20">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="AE4" s="18"/>
       <c r="AF4" t="s" s="20">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="AG4" s="18"/>
       <c r="AH4" t="s" s="20">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="AI4" s="18"/>
       <c r="AJ4" t="s" s="20">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="AK4" s="18"/>
       <c r="AL4" t="s" s="20">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="AM4" s="18"/>
       <c r="AN4" t="s" s="20">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="AO4" t="s" s="20">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="AP4" s="18"/>
       <c r="AQ4" t="s" s="20">
+        <v>97</v>
+      </c>
+      <c r="AR4" t="s" s="20">
+        <v>96</v>
+      </c>
+      <c r="AS4" t="s" s="21">
         <v>98</v>
       </c>
-      <c r="AR4" t="s" s="20">
-        <v>97</v>
-      </c>
-      <c r="AS4" t="s" s="21">
+      <c r="AT4" t="s" s="20">
         <v>99</v>
-      </c>
-      <c r="AT4" t="s" s="20">
-        <v>100</v>
       </c>
       <c r="AU4" s="18"/>
       <c r="AV4" t="s" s="20">
-        <v>35</v>
+        <v>100</v>
       </c>
       <c r="AW4" t="s" s="20">
         <v>101</v>
       </c>
       <c r="AX4" t="s" s="21">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AY4" t="s" s="20">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AZ4" s="18"/>
       <c r="BA4" t="s" s="20">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="BB4" t="s" s="20">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="BC4" s="18"/>
       <c r="BD4" t="s" s="20">
-        <v>99</v>
-      </c>
+        <v>98</v>
+      </c>
+    </row>
+    <row r="5" ht="14.05" customHeight="1">
+      <c r="A5" s="22"/>
+      <c r="B5" s="23"/>
+      <c r="C5" s="23"/>
+      <c r="D5" s="23"/>
+      <c r="E5" s="23"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="23"/>
+      <c r="H5" s="23"/>
+      <c r="I5" s="23"/>
+      <c r="J5" s="23"/>
+      <c r="K5" s="23"/>
+      <c r="L5" s="4"/>
+      <c r="M5" s="23"/>
+      <c r="N5" s="23"/>
+      <c r="O5" s="23"/>
+      <c r="P5" s="23"/>
+      <c r="Q5" s="4"/>
+      <c r="R5" s="4"/>
+      <c r="S5" s="4"/>
+      <c r="T5" s="4"/>
+      <c r="U5" s="4"/>
+      <c r="V5" s="4"/>
+      <c r="W5" s="4"/>
+      <c r="X5" s="4"/>
+      <c r="Y5" s="4"/>
+      <c r="Z5" s="4"/>
+      <c r="AA5" s="4"/>
+      <c r="AB5" s="23"/>
+      <c r="AC5" s="4"/>
+      <c r="AD5" s="23"/>
+      <c r="AE5" s="4"/>
+      <c r="AF5" s="23"/>
+      <c r="AG5" s="4"/>
+      <c r="AH5" s="23"/>
+      <c r="AI5" s="4"/>
+      <c r="AJ5" s="23"/>
+      <c r="AK5" s="4"/>
+      <c r="AL5" s="23"/>
+      <c r="AM5" s="4"/>
+      <c r="AN5" s="23"/>
+      <c r="AO5" s="23"/>
+      <c r="AP5" s="4"/>
+      <c r="AQ5" s="23"/>
+      <c r="AR5" s="23"/>
+      <c r="AS5" s="23"/>
+      <c r="AT5" s="23"/>
+      <c r="AU5" s="4"/>
+      <c r="AV5" s="23"/>
+      <c r="AW5" s="23"/>
+      <c r="AX5" s="23"/>
+      <c r="AY5" s="23"/>
+      <c r="AZ5" s="4"/>
+      <c r="BA5" s="23"/>
+      <c r="BB5" s="23"/>
+      <c r="BC5" s="4"/>
+      <c r="BD5" s="24"/>
+    </row>
+    <row r="6" ht="13.55" customHeight="1">
+      <c r="A6" s="25"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="8"/>
+      <c r="J6" s="8"/>
+      <c r="K6" s="8"/>
+      <c r="L6" s="8"/>
+      <c r="M6" s="8"/>
+      <c r="N6" s="8"/>
+      <c r="O6" s="8"/>
+      <c r="P6" s="8"/>
+      <c r="Q6" s="8"/>
+      <c r="R6" s="8"/>
+      <c r="S6" s="8"/>
+      <c r="T6" s="8"/>
+      <c r="U6" s="8"/>
+      <c r="V6" s="8"/>
+      <c r="W6" s="8"/>
+      <c r="X6" s="8"/>
+      <c r="Y6" s="8"/>
+      <c r="Z6" s="8"/>
+      <c r="AA6" s="8"/>
+      <c r="AB6" s="8"/>
+      <c r="AC6" s="8"/>
+      <c r="AD6" s="8"/>
+      <c r="AE6" s="8"/>
+      <c r="AF6" s="8"/>
+      <c r="AG6" s="8"/>
+      <c r="AH6" s="8"/>
+      <c r="AI6" s="8"/>
+      <c r="AJ6" s="8"/>
+      <c r="AK6" s="8"/>
+      <c r="AL6" s="8"/>
+      <c r="AM6" s="8"/>
+      <c r="AN6" s="8"/>
+      <c r="AO6" s="8"/>
+      <c r="AP6" s="8"/>
+      <c r="AQ6" s="8"/>
+      <c r="AR6" s="8"/>
+      <c r="AS6" s="8"/>
+      <c r="AT6" s="8"/>
+      <c r="AU6" s="8"/>
+      <c r="AV6" s="8"/>
+      <c r="AW6" s="8"/>
+      <c r="AX6" s="8"/>
+      <c r="AY6" s="8"/>
+      <c r="AZ6" s="8"/>
+      <c r="BA6" s="8"/>
+      <c r="BB6" s="8"/>
+      <c r="BC6" s="8"/>
+      <c r="BD6" s="9"/>
+    </row>
+    <row r="7" ht="13.55" customHeight="1">
+      <c r="A7" s="25"/>
+      <c r="B7" s="8"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="8"/>
+      <c r="K7" s="8"/>
+      <c r="L7" s="8"/>
+      <c r="M7" s="8"/>
+      <c r="N7" s="8"/>
+      <c r="O7" s="8"/>
+      <c r="P7" s="8"/>
+      <c r="Q7" s="8"/>
+      <c r="R7" s="8"/>
+      <c r="S7" s="8"/>
+      <c r="T7" s="8"/>
+      <c r="U7" s="8"/>
+      <c r="V7" s="8"/>
+      <c r="W7" s="8"/>
+      <c r="X7" s="8"/>
+      <c r="Y7" s="8"/>
+      <c r="Z7" s="8"/>
+      <c r="AA7" s="8"/>
+      <c r="AB7" s="8"/>
+      <c r="AC7" s="8"/>
+      <c r="AD7" s="8"/>
+      <c r="AE7" s="8"/>
+      <c r="AF7" s="8"/>
+      <c r="AG7" s="8"/>
+      <c r="AH7" s="8"/>
+      <c r="AI7" s="8"/>
+      <c r="AJ7" s="8"/>
+      <c r="AK7" s="8"/>
+      <c r="AL7" s="8"/>
+      <c r="AM7" s="8"/>
+      <c r="AN7" s="8"/>
+      <c r="AO7" s="8"/>
+      <c r="AP7" s="8"/>
+      <c r="AQ7" s="8"/>
+      <c r="AR7" s="8"/>
+      <c r="AS7" s="8"/>
+      <c r="AT7" s="8"/>
+      <c r="AU7" s="8"/>
+      <c r="AV7" s="8"/>
+      <c r="AW7" s="8"/>
+      <c r="AX7" s="8"/>
+      <c r="AY7" s="8"/>
+      <c r="AZ7" s="8"/>
+      <c r="BA7" s="8"/>
+      <c r="BB7" s="8"/>
+      <c r="BC7" s="8"/>
+      <c r="BD7" s="9"/>
+    </row>
+    <row r="8" ht="13.55" customHeight="1">
+      <c r="A8" s="25"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="8"/>
+      <c r="J8" s="8"/>
+      <c r="K8" s="8"/>
+      <c r="L8" s="8"/>
+      <c r="M8" s="8"/>
+      <c r="N8" s="8"/>
+      <c r="O8" s="8"/>
+      <c r="P8" s="8"/>
+      <c r="Q8" s="8"/>
+      <c r="R8" s="8"/>
+      <c r="S8" s="8"/>
+      <c r="T8" s="8"/>
+      <c r="U8" s="8"/>
+      <c r="V8" s="8"/>
+      <c r="W8" s="8"/>
+      <c r="X8" s="8"/>
+      <c r="Y8" s="8"/>
+      <c r="Z8" s="8"/>
+      <c r="AA8" s="8"/>
+      <c r="AB8" s="8"/>
+      <c r="AC8" s="8"/>
+      <c r="AD8" s="8"/>
+      <c r="AE8" s="8"/>
+      <c r="AF8" s="8"/>
+      <c r="AG8" s="8"/>
+      <c r="AH8" s="8"/>
+      <c r="AI8" s="8"/>
+      <c r="AJ8" s="8"/>
+      <c r="AK8" s="8"/>
+      <c r="AL8" s="8"/>
+      <c r="AM8" s="8"/>
+      <c r="AN8" s="8"/>
+      <c r="AO8" s="8"/>
+      <c r="AP8" s="8"/>
+      <c r="AQ8" s="8"/>
+      <c r="AR8" s="8"/>
+      <c r="AS8" s="8"/>
+      <c r="AT8" s="8"/>
+      <c r="AU8" s="8"/>
+      <c r="AV8" s="8"/>
+      <c r="AW8" s="8"/>
+      <c r="AX8" s="8"/>
+      <c r="AY8" s="8"/>
+      <c r="AZ8" s="8"/>
+      <c r="BA8" s="8"/>
+      <c r="BB8" s="8"/>
+      <c r="BC8" s="8"/>
+      <c r="BD8" s="9"/>
+    </row>
+    <row r="9" ht="13.55" customHeight="1">
+      <c r="A9" s="25"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="8"/>
+      <c r="J9" s="8"/>
+      <c r="K9" s="8"/>
+      <c r="L9" s="8"/>
+      <c r="M9" s="8"/>
+      <c r="N9" s="8"/>
+      <c r="O9" s="8"/>
+      <c r="P9" s="8"/>
+      <c r="Q9" s="8"/>
+      <c r="R9" s="8"/>
+      <c r="S9" s="8"/>
+      <c r="T9" s="8"/>
+      <c r="U9" s="8"/>
+      <c r="V9" s="8"/>
+      <c r="W9" s="8"/>
+      <c r="X9" s="8"/>
+      <c r="Y9" s="8"/>
+      <c r="Z9" s="8"/>
+      <c r="AA9" s="8"/>
+      <c r="AB9" s="8"/>
+      <c r="AC9" s="8"/>
+      <c r="AD9" s="8"/>
+      <c r="AE9" s="8"/>
+      <c r="AF9" s="8"/>
+      <c r="AG9" s="8"/>
+      <c r="AH9" s="8"/>
+      <c r="AI9" s="8"/>
+      <c r="AJ9" s="8"/>
+      <c r="AK9" s="8"/>
+      <c r="AL9" s="8"/>
+      <c r="AM9" s="8"/>
+      <c r="AN9" s="8"/>
+      <c r="AO9" s="8"/>
+      <c r="AP9" s="8"/>
+      <c r="AQ9" s="8"/>
+      <c r="AR9" s="8"/>
+      <c r="AS9" s="8"/>
+      <c r="AT9" s="8"/>
+      <c r="AU9" s="8"/>
+      <c r="AV9" s="8"/>
+      <c r="AW9" s="8"/>
+      <c r="AX9" s="8"/>
+      <c r="AY9" s="8"/>
+      <c r="AZ9" s="8"/>
+      <c r="BA9" s="8"/>
+      <c r="BB9" s="8"/>
+      <c r="BC9" s="8"/>
+      <c r="BD9" s="9"/>
+    </row>
+    <row r="10" ht="13.55" customHeight="1">
+      <c r="A10" s="26"/>
+      <c r="B10" s="13"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="13"/>
+      <c r="I10" s="13"/>
+      <c r="J10" s="13"/>
+      <c r="K10" s="13"/>
+      <c r="L10" s="13"/>
+      <c r="M10" s="13"/>
+      <c r="N10" s="13"/>
+      <c r="O10" s="13"/>
+      <c r="P10" s="13"/>
+      <c r="Q10" s="13"/>
+      <c r="R10" s="13"/>
+      <c r="S10" s="13"/>
+      <c r="T10" s="13"/>
+      <c r="U10" s="13"/>
+      <c r="V10" s="13"/>
+      <c r="W10" s="13"/>
+      <c r="X10" s="13"/>
+      <c r="Y10" s="13"/>
+      <c r="Z10" s="13"/>
+      <c r="AA10" s="13"/>
+      <c r="AB10" s="13"/>
+      <c r="AC10" s="13"/>
+      <c r="AD10" s="13"/>
+      <c r="AE10" s="13"/>
+      <c r="AF10" s="13"/>
+      <c r="AG10" s="13"/>
+      <c r="AH10" s="13"/>
+      <c r="AI10" s="13"/>
+      <c r="AJ10" s="13"/>
+      <c r="AK10" s="13"/>
+      <c r="AL10" s="13"/>
+      <c r="AM10" s="13"/>
+      <c r="AN10" s="13"/>
+      <c r="AO10" s="13"/>
+      <c r="AP10" s="13"/>
+      <c r="AQ10" s="13"/>
+      <c r="AR10" s="13"/>
+      <c r="AS10" s="13"/>
+      <c r="AT10" s="13"/>
+      <c r="AU10" s="13"/>
+      <c r="AV10" s="13"/>
+      <c r="AW10" s="13"/>
+      <c r="AX10" s="13"/>
+      <c r="AY10" s="13"/>
+      <c r="AZ10" s="13"/>
+      <c r="BA10" s="13"/>
+      <c r="BB10" s="13"/>
+      <c r="BC10" s="13"/>
+      <c r="BD10" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2552,19 +2962,19 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="6" width="20" style="22" customWidth="1"/>
-    <col min="7" max="16384" width="8.85156" style="22" customWidth="1"/>
+    <col min="1" max="6" width="20" style="27" customWidth="1"/>
+    <col min="7" max="16384" width="8.85156" style="27" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="20" customHeight="1">
-      <c r="A1" t="s" s="23">
+      <c r="A1" t="s" s="28">
         <v>102</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
     </row>
     <row r="2" ht="13.55" customHeight="1">
       <c r="A2" t="s" s="19">
@@ -2582,25 +2992,25 @@
       <c r="E2" t="s" s="19">
         <v>107</v>
       </c>
-      <c r="F2" t="s" s="25">
+      <c r="F2" t="s" s="30">
         <v>108</v>
       </c>
     </row>
     <row r="3" ht="10" customHeight="1">
-      <c r="A3" s="26"/>
-      <c r="B3" s="26"/>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26"/>
-      <c r="F3" s="27"/>
+      <c r="A3" s="31"/>
+      <c r="B3" s="31"/>
+      <c r="C3" s="31"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="31"/>
+      <c r="F3" s="32"/>
     </row>
     <row r="4" ht="14.05" customHeight="1">
-      <c r="A4" s="28"/>
-      <c r="B4" s="28"/>
-      <c r="C4" s="28"/>
-      <c r="D4" s="28"/>
-      <c r="E4" s="28"/>
-      <c r="F4" s="29"/>
+      <c r="A4" s="33"/>
+      <c r="B4" s="33"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="34"/>
     </row>
     <row r="5" ht="13.55" customHeight="1">
       <c r="A5" s="18"/>
@@ -2608,7 +3018,7 @@
       <c r="C5" s="18"/>
       <c r="D5" s="18"/>
       <c r="E5" s="18"/>
-      <c r="F5" s="30"/>
+      <c r="F5" s="35"/>
     </row>
     <row r="6" ht="13.55" customHeight="1">
       <c r="A6" s="18"/>
@@ -2616,7 +3026,7 @@
       <c r="C6" s="18"/>
       <c r="D6" s="18"/>
       <c r="E6" s="18"/>
-      <c r="F6" s="30"/>
+      <c r="F6" s="35"/>
     </row>
     <row r="7" ht="13.55" customHeight="1">
       <c r="A7" s="18"/>
@@ -2624,7 +3034,7 @@
       <c r="C7" s="18"/>
       <c r="D7" s="18"/>
       <c r="E7" s="18"/>
-      <c r="F7" s="30"/>
+      <c r="F7" s="35"/>
     </row>
     <row r="8" ht="13.55" customHeight="1">
       <c r="A8" s="18"/>
@@ -2632,7 +3042,7 @@
       <c r="C8" s="18"/>
       <c r="D8" s="18"/>
       <c r="E8" s="18"/>
-      <c r="F8" s="30"/>
+      <c r="F8" s="35"/>
     </row>
     <row r="9" ht="13.55" customHeight="1">
       <c r="A9" s="18"/>
@@ -2640,7 +3050,7 @@
       <c r="C9" s="18"/>
       <c r="D9" s="18"/>
       <c r="E9" s="18"/>
-      <c r="F9" s="30"/>
+      <c r="F9" s="35"/>
     </row>
     <row r="10" ht="13.55" customHeight="1">
       <c r="A10" s="18"/>
@@ -2648,7 +3058,7 @@
       <c r="C10" s="18"/>
       <c r="D10" s="18"/>
       <c r="E10" s="18"/>
-      <c r="F10" s="30"/>
+      <c r="F10" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>